<commit_message>
Atualizando o arquivo APP.xlsx
</commit_message>
<xml_diff>
--- a/APP.xlsx
+++ b/APP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabrina.marcandali\Desktop\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\meu-projeto\Pratica R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51E8F42-B736-4812-91C3-7BF2006D9C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E147D46-DC3B-4BED-ACE0-BAD4172D43E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0E938952-A300-4F9C-9C66-F1A8D20E7C13}"/>
   </bookViews>

</xml_diff>